<commit_message>
Add new QC folders and files
</commit_message>
<xml_diff>
--- a/California/Belridge_South/completion/403056866/logs/TreatmentStages_0403056866.xlsx
+++ b/California/Belridge_South/completion/403056866/logs/TreatmentStages_0403056866.xlsx
@@ -763,8 +763,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A77FC0EA97D2041BFDF7421B1DCA700" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4d671ce28fcc8db05849f288d506af22">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36620a0f-9544-4c16-8d33-3543000407f5" xmlns:ns3="20093c4f-14af-4980-b708-d2dd3420b9c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="168cc6fbf8d6e6f4846569bb2f02a81c" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A77FC0EA97D2041BFDF7421B1DCA700" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8442bf5ddf19e33433c6920e5ef5dfd3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="36620a0f-9544-4c16-8d33-3543000407f5" xmlns:ns3="20093c4f-14af-4980-b708-d2dd3420b9c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="523c1699faaf49aacdce22b312f39cf8" ns1:_="" ns2:_="" ns3:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="36620a0f-9544-4c16-8d33-3543000407f5"/>
     <xsd:import namespace="20093c4f-14af-4980-b708-d2dd3420b9c6"/>
     <xsd:element name="properties">
@@ -786,11 +787,27 @@
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="22" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="23" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="36620a0f-9544-4c16-8d33-3543000407f5" elementFormDefault="qualified">
@@ -1000,12 +1017,14 @@
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="36620a0f-9544-4c16-8d33-3543000407f5">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6188E934-C3B6-473C-9C16-2387CD4F4064}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{581E313F-FD1A-4F5E-9E9A-E6DFF38E10E2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>